<commit_message>
Precedents + Valuation Overview
</commit_message>
<xml_diff>
--- a/models/Comps_Precs.xlsx
+++ b/models/Comps_Precs.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cb10f4a09bcef627/Documents/GitHub/XD_Grad_Portfolio/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="516" documentId="8_{03E98026-E5C0-4EE9-B1A4-ED0B6BC034C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{283D1A5D-B541-4462-A413-8B5B7E5A93A9}"/>
+  <xr:revisionPtr revIDLastSave="814" documentId="8_{03E98026-E5C0-4EE9-B1A4-ED0B6BC034C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4433886C-081E-4B0B-8D7E-757F4A247425}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6F36A4A9-635C-494E-BE77-27E5FD1262DF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{6F36A4A9-635C-494E-BE77-27E5FD1262DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparable Companies" sheetId="1" r:id="rId1"/>
+    <sheet name="Precedent Transactions" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
     <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -93,12 +94,136 @@
         </r>
       </text>
     </comment>
+    <comment ref="J29" authorId="0" shapeId="0" xr:uid="{FE4C1B06-8D6C-4DF8-AF9F-0BBE3129AE44}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xavier Davis:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Usually would use average of harmonic mean and median but due to mean not showing too heavy kurtosis
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Xavier Davis</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{3119AFBE-D221-4DEE-8128-6137349A7A10}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xavier Davis: 
+All data using LTM at announcement date, non inflation adjusted</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{CD536EC1-43CA-4401-8F0E-355DE0A04E52}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xavier Davis:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+private company, non disclosed for deal period
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{7A534839-A76C-4FC2-8096-B3860EC0A3C7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xavier Davis:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+EBIT only 9 month published in 2016 for some reason</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{A115C98E-7F94-4305-AF39-56F6FCBEB086}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xavier Davis:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+ridiculously high D&amp;A has been validated, this data point has been excluded
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="66">
   <si>
     <t>Stryker</t>
   </si>
@@ -220,19 +345,95 @@
     <t>Price Difference:</t>
   </si>
   <si>
-    <t>Implied Ordinary Share Price</t>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Buyer</t>
+  </si>
+  <si>
+    <t>Valuation Metrics</t>
+  </si>
+  <si>
+    <t>EV/Sales</t>
+  </si>
+  <si>
+    <t>EV/EBITDA</t>
+  </si>
+  <si>
+    <t>EV/EBIT</t>
+  </si>
+  <si>
+    <t>Acelity</t>
+  </si>
+  <si>
+    <t>BSN Medical</t>
+  </si>
+  <si>
+    <t>Wright Medical</t>
+  </si>
+  <si>
+    <t>Hillrom</t>
+  </si>
+  <si>
+    <t>ArthroCare</t>
+  </si>
+  <si>
+    <t>Transaction Value ($MM)</t>
+  </si>
+  <si>
+    <t>EUR/USD</t>
+  </si>
+  <si>
+    <t>3M</t>
+  </si>
+  <si>
+    <t>Essity (formerly SCA)</t>
+  </si>
+  <si>
+    <t>Baxter</t>
+  </si>
+  <si>
+    <t>Smith &amp; Nephew</t>
+  </si>
+  <si>
+    <t>Relative Valuation</t>
+  </si>
+  <si>
+    <t>Share Price</t>
+  </si>
+  <si>
+    <t>Implied EV</t>
+  </si>
+  <si>
+    <t>Net Debt</t>
+  </si>
+  <si>
+    <t>Implied Share Price</t>
+  </si>
+  <si>
+    <t>Implied  Share Price</t>
+  </si>
+  <si>
+    <t>Average of Averages</t>
+  </si>
+  <si>
+    <t>N/D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.00;[Red]0.00;\-"/>
-    <numFmt numFmtId="171" formatCode="0;\(0\);\-"/>
-    <numFmt numFmtId="173" formatCode="0.00;\(0.00\);\-"/>
+    <numFmt numFmtId="165" formatCode="0;\(0\);\-"/>
+    <numFmt numFmtId="166" formatCode="0.00;\(0.00\);\-"/>
+    <numFmt numFmtId="168" formatCode="#,##0.00&quot;x&quot;"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -321,8 +522,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u val="singleAccounting"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -361,6 +585,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -403,7 +633,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -420,21 +650,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="10" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="10" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -462,9 +687,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="173" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="13" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="12" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,8 +747,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -879,15 +1123,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DB3578-96B1-4D7B-B55B-1582E36903A2}">
-  <dimension ref="B2:Q32"/>
+  <dimension ref="B2:Q33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+    <sheetView showGridLines="0" zoomScale="93" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3:Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
@@ -976,51 +1220,51 @@
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="14">
         <v>364.43</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="13">
         <v>139370</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="13">
         <v>152880</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="13">
         <v>386</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="13">
         <v>22595</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="13">
         <v>6006</v>
       </c>
-      <c r="I4" s="18">
+      <c r="I4" s="13">
         <v>4956</v>
       </c>
-      <c r="J4" s="18">
+      <c r="J4" s="13">
         <v>2993</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="35">
         <f>E4/G4</f>
         <v>6.7660986944014159</v>
       </c>
-      <c r="L4" s="9">
+      <c r="L4" s="35">
         <f>E4/H4</f>
         <v>25.454545454545453</v>
       </c>
-      <c r="M4" s="9">
+      <c r="M4" s="35">
         <f>E4/I4</f>
         <v>30.847457627118644</v>
       </c>
-      <c r="N4" s="9">
+      <c r="N4" s="35">
         <f>C4/O4</f>
         <v>46.99965920481123</v>
       </c>
-      <c r="O4" s="9">
-        <f>J4/F4</f>
+      <c r="O4" s="35">
+        <f t="shared" ref="O4:O9" si="0">J4/F4</f>
         <v>7.7538860103626943</v>
       </c>
     </row>
@@ -1028,48 +1272,48 @@
       <c r="B5" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="14">
         <v>88.35</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="13">
         <v>17510</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="13">
         <v>24470</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="13">
         <v>204</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="13">
         <v>7679</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="13">
         <v>2590</v>
       </c>
-      <c r="I5" s="18">
+      <c r="I5" s="13">
         <v>1594</v>
       </c>
-      <c r="J5" s="18">
+      <c r="J5" s="13">
         <v>903.8</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="35">
         <f>E5/G5</f>
         <v>3.1866128402135696</v>
       </c>
-      <c r="L5" s="9">
+      <c r="L5" s="35">
         <f>E5/H5</f>
         <v>9.4478764478764479</v>
       </c>
-      <c r="M5" s="9">
+      <c r="M5" s="35">
         <f>E5/I5</f>
         <v>15.351317440401505</v>
       </c>
-      <c r="N5" s="9">
+      <c r="N5" s="35">
         <f>C5/O5</f>
         <v>19.941801283469797</v>
       </c>
-      <c r="O5" s="9">
-        <f>J5/F5</f>
+      <c r="O5" s="35">
+        <f t="shared" si="0"/>
         <v>4.4303921568627445</v>
       </c>
     </row>
@@ -1077,48 +1321,48 @@
       <c r="B6" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="14">
         <v>194.15</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="13">
         <v>466580</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="13">
         <v>494230</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="13">
         <v>2429</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="13">
         <v>88821</v>
       </c>
-      <c r="H6" s="18">
+      <c r="H6" s="13">
         <v>29940</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="13">
         <v>22601</v>
       </c>
-      <c r="J6" s="18">
+      <c r="J6" s="13">
         <v>14066</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K6" s="35">
         <f>E6/G6</f>
         <v>5.5643372625842984</v>
       </c>
-      <c r="L6" s="9">
+      <c r="L6" s="35">
         <f>E6/H6</f>
         <v>16.507348029392119</v>
       </c>
-      <c r="M6" s="9">
+      <c r="M6" s="35">
         <f>E6/I6</f>
         <v>21.867616477147028</v>
       </c>
-      <c r="N6" s="9">
+      <c r="N6" s="35">
         <f>C6/O6</f>
         <v>33.526969287643965</v>
       </c>
-      <c r="O6" s="9">
-        <f>J6/F6</f>
+      <c r="O6" s="35">
+        <f t="shared" si="0"/>
         <v>5.7908604363935776</v>
       </c>
     </row>
@@ -1126,55 +1370,55 @@
       <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="14">
         <f>600.4*Q3</f>
         <v>96.063999999999993</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="13">
         <f>16000*Q2</f>
         <v>20800</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="13">
         <f>18560*Q2</f>
         <v>24128</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="13">
         <v>225</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="13">
         <f>27874*Q3</f>
         <v>4459.84</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="13">
         <f>8630*Q3</f>
         <v>1380.8</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="13">
         <f>7721*Q3</f>
         <v>1235.3600000000001</v>
       </c>
-      <c r="J7" s="18">
+      <c r="J7" s="13">
         <f>3636*Q3</f>
         <v>581.76</v>
       </c>
-      <c r="K7" s="9">
+      <c r="K7" s="35">
         <f>E7/G7</f>
         <v>5.4100595537059624</v>
       </c>
-      <c r="L7" s="9">
+      <c r="L7" s="35">
         <f>E7/H7</f>
         <v>17.473928157589803</v>
       </c>
-      <c r="M7" s="9">
+      <c r="M7" s="35">
         <f>E7/I7</f>
         <v>19.531148814920346</v>
       </c>
-      <c r="N7" s="9">
+      <c r="N7" s="35">
         <f>C7/O7</f>
         <v>37.153465346534652</v>
       </c>
-      <c r="O7" s="9">
-        <f>J7/F7</f>
+      <c r="O7" s="35">
+        <f t="shared" si="0"/>
         <v>2.5855999999999999</v>
       </c>
     </row>
@@ -1182,55 +1426,55 @@
       <c r="B8" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="14">
         <f>236.4/100*Q2</f>
         <v>3.0731999999999999</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="13">
         <f>4660*Q2</f>
         <v>6058</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="13">
         <f>5570*Q2</f>
         <v>7241</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="13">
         <v>2057</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="13">
         <f>2289</f>
         <v>2289</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="13">
         <f>527.9</f>
         <v>527.9</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I8" s="13">
         <f>350.7</f>
         <v>350.7</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="13">
         <f>190.5</f>
         <v>190.5</v>
       </c>
-      <c r="K8" s="9">
+      <c r="K8" s="35">
         <f>E8/G8</f>
         <v>3.163390126692879</v>
       </c>
-      <c r="L8" s="9">
+      <c r="L8" s="35">
         <f>E8/H8</f>
         <v>13.716612994885395</v>
       </c>
-      <c r="M8" s="9">
+      <c r="M8" s="35">
         <f>E8/I8</f>
         <v>20.647276874821785</v>
       </c>
-      <c r="N8" s="9">
+      <c r="N8" s="35">
         <f>C8/O8</f>
         <v>33.184107086614169</v>
       </c>
-      <c r="O8" s="9">
-        <f>J8/F8</f>
+      <c r="O8" s="35">
+        <f t="shared" si="0"/>
         <v>9.2610597958191543E-2</v>
       </c>
     </row>
@@ -1238,242 +1482,242 @@
       <c r="B9" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="14">
         <f>[1]DCF!$I$9</f>
         <v>36.82</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18">
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13">
         <f>'[2]Income Statement'!$F$25</f>
         <v>876</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="13">
         <f>'[2]Income Statement'!$F$2</f>
         <v>5810</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="13">
         <f>'[2]Income Statement'!$F$40</f>
         <v>1335</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="13">
         <f>'[2]Income Statement'!$F$8</f>
         <v>886</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="13">
         <f>'[2]Income Statement'!$F$21</f>
         <v>412</v>
       </c>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9">
-        <f>J9/F9</f>
+      <c r="K9" s="35"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="35"/>
+      <c r="O9" s="35">
+        <f t="shared" si="0"/>
         <v>0.47031963470319632</v>
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="15">
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="36">
         <f>MIN(K4:K8)</f>
         <v>3.163390126692879</v>
       </c>
-      <c r="L10" s="15">
-        <f t="shared" ref="L10:M10" si="0">MIN(L4:L8)</f>
+      <c r="L10" s="36">
+        <f>MIN(L4:L8)</f>
         <v>9.4478764478764479</v>
       </c>
-      <c r="M10" s="15">
-        <f t="shared" si="0"/>
+      <c r="M10" s="36">
+        <f>MIN(M4:M8)</f>
         <v>15.351317440401505</v>
       </c>
-      <c r="N10" s="15">
+      <c r="N10" s="36">
         <f>MIN(N4:N8)</f>
         <v>19.941801283469797</v>
       </c>
-      <c r="O10" s="15">
+      <c r="O10" s="36">
         <f>MIN(O4:O8)</f>
         <v>9.2610597958191543E-2</v>
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="16">
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="36">
         <f>_xlfn.PERCENTILE.INC(K4:K8,0.25)</f>
         <v>3.1866128402135696</v>
       </c>
-      <c r="L11" s="16">
-        <f t="shared" ref="L11:O11" si="1">_xlfn.PERCENTILE.INC(L4:L8,0.25)</f>
+      <c r="L11" s="36">
+        <f>_xlfn.PERCENTILE.INC(L4:L8,0.25)</f>
         <v>13.716612994885395</v>
       </c>
-      <c r="M11" s="16">
-        <f t="shared" si="1"/>
+      <c r="M11" s="36">
+        <f>_xlfn.PERCENTILE.INC(M4:M8,0.25)</f>
         <v>19.531148814920346</v>
       </c>
-      <c r="N11" s="16">
-        <f t="shared" si="1"/>
+      <c r="N11" s="36">
+        <f>_xlfn.PERCENTILE.INC(N4:N8,0.25)</f>
         <v>33.184107086614169</v>
       </c>
-      <c r="O11" s="16">
-        <f t="shared" si="1"/>
+      <c r="O11" s="36">
+        <f>_xlfn.PERCENTILE.INC(O4:O8,0.25)</f>
         <v>2.5855999999999999</v>
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="13">
+      <c r="C12" s="9"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="37">
         <f>MEDIAN(K4:K8)</f>
         <v>5.4100595537059624</v>
       </c>
-      <c r="L12" s="13">
+      <c r="L12" s="37">
         <f>MEDIAN(L4:L8)</f>
         <v>16.507348029392119</v>
       </c>
-      <c r="M12" s="13">
+      <c r="M12" s="37">
         <f>MEDIAN(M4:M8)</f>
         <v>20.647276874821785</v>
       </c>
-      <c r="N12" s="13">
+      <c r="N12" s="37">
         <f>MEDIAN(N4:N8)</f>
         <v>33.526969287643965</v>
       </c>
-      <c r="O12" s="13">
+      <c r="O12" s="37">
         <f>MEDIAN(O4:O8)</f>
         <v>4.4303921568627445</v>
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="37">
+        <f>HARMEAN(K4:K8)</f>
+        <v>4.3772035255364559</v>
+      </c>
+      <c r="L13" s="37">
+        <f>HARMEAN(L4:L8)</f>
+        <v>14.887993202058716</v>
+      </c>
+      <c r="M13" s="37">
+        <f>HARMEAN(M4:M8)</f>
+        <v>20.582815210404071</v>
+      </c>
+      <c r="N13" s="37">
+        <f>HARMEAN(N4:N8)</f>
+        <v>31.585656247129439</v>
+      </c>
+      <c r="O13" s="37">
+        <f>HARMEAN(O4:O8)</f>
+        <v>0.42691166279533649</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B14" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="14">
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="37">
         <f>AVERAGE(K4:K8)</f>
         <v>4.8180996955196251</v>
       </c>
-      <c r="L13" s="14">
+      <c r="L14" s="37">
         <f>AVERAGE(L4:L8)</f>
         <v>16.520062216857845</v>
       </c>
-      <c r="M13" s="14">
+      <c r="M14" s="37">
         <f>AVERAGE(M4:M8)</f>
         <v>21.648963446881858</v>
       </c>
-      <c r="N13" s="14">
+      <c r="N14" s="37">
         <f>AVERAGE(N4:N8)</f>
         <v>34.161200441814763</v>
       </c>
-      <c r="O13" s="14">
+      <c r="O14" s="37">
         <f>AVERAGE(O4:O8)</f>
         <v>4.1306698403154414</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B14" s="11" t="s">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B15" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="16">
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="36">
         <f>_xlfn.PERCENTILE.INC(K4:K8,0.75)</f>
         <v>5.5643372625842984</v>
       </c>
-      <c r="L14" s="16">
-        <f t="shared" ref="L14:O14" si="2">_xlfn.PERCENTILE.INC(L4:L8,0.75)</f>
+      <c r="L15" s="36">
+        <f>_xlfn.PERCENTILE.INC(L4:L8,0.75)</f>
         <v>17.473928157589803</v>
       </c>
-      <c r="M14" s="16">
-        <f t="shared" si="2"/>
+      <c r="M15" s="36">
+        <f>_xlfn.PERCENTILE.INC(M4:M8,0.75)</f>
         <v>21.867616477147028</v>
       </c>
-      <c r="N14" s="16">
-        <f t="shared" si="2"/>
+      <c r="N15" s="36">
+        <f>_xlfn.PERCENTILE.INC(N4:N8,0.75)</f>
         <v>37.153465346534652</v>
       </c>
-      <c r="O14" s="16">
-        <f t="shared" si="2"/>
+      <c r="O15" s="36">
+        <f>_xlfn.PERCENTILE.INC(O4:O8,0.75)</f>
         <v>5.7908604363935776</v>
-      </c>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B15" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="15">
-        <f>MAX(K4:K8)</f>
-        <v>6.7660986944014159</v>
-      </c>
-      <c r="L15" s="15">
-        <f t="shared" ref="L15:O15" si="3">MAX(L4:L8)</f>
-        <v>25.454545454545453</v>
-      </c>
-      <c r="M15" s="15">
-        <f t="shared" si="3"/>
-        <v>30.847457627118644</v>
-      </c>
-      <c r="N15" s="15">
-        <f t="shared" si="3"/>
-        <v>46.99965920481123</v>
-      </c>
-      <c r="O15" s="15">
-        <f t="shared" si="3"/>
-        <v>7.7538860103626943</v>
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B16" s="10" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -1483,25 +1727,25 @@
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
-      <c r="K16" s="21">
-        <f>HARMEAN(K4:K8)</f>
-        <v>4.3772035255364559</v>
-      </c>
-      <c r="L16" s="21">
-        <f t="shared" ref="L16:O16" si="4">HARMEAN(L4:L8)</f>
-        <v>14.887993202058716</v>
-      </c>
-      <c r="M16" s="21">
-        <f t="shared" si="4"/>
-        <v>20.582815210404071</v>
-      </c>
-      <c r="N16" s="21">
-        <f t="shared" si="4"/>
-        <v>31.585656247129439</v>
-      </c>
-      <c r="O16" s="21">
-        <f t="shared" si="4"/>
-        <v>0.42691166279533649</v>
+      <c r="K16" s="36">
+        <f>MAX(K4:K8)</f>
+        <v>6.7660986944014159</v>
+      </c>
+      <c r="L16" s="36">
+        <f>MAX(L4:L8)</f>
+        <v>25.454545454545453</v>
+      </c>
+      <c r="M16" s="36">
+        <f>MAX(M4:M8)</f>
+        <v>30.847457627118644</v>
+      </c>
+      <c r="N16" s="36">
+        <f>MAX(N4:N8)</f>
+        <v>46.99965920481123</v>
+      </c>
+      <c r="O16" s="36">
+        <f>MAX(O4:O8)</f>
+        <v>7.7538860103626943</v>
       </c>
     </row>
     <row r="17" spans="2:15" ht="16.2" x14ac:dyDescent="0.45">
@@ -1516,393 +1760,963 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-      <c r="K17" s="32" t="s">
+      <c r="K17" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="21"/>
+      <c r="O17" s="21"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="17">
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="12">
         <f>K12*G9</f>
         <v>31432.446007031642</v>
       </c>
-      <c r="L18" s="17">
+      <c r="L18" s="12">
         <f>L12*$H$9</f>
         <v>22037.30961923848</v>
       </c>
-      <c r="M18" s="17">
+      <c r="M18" s="12">
         <f>M12*$I$9</f>
         <v>18293.4873110921</v>
       </c>
-      <c r="N18" s="17">
+      <c r="N18" s="12">
         <f>N22-C19</f>
         <v>27626.222693018626</v>
       </c>
-      <c r="O18" s="21"/>
+      <c r="O18" s="16"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="17">
-        <f>K13*G9</f>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="12">
+        <f>K14*G9</f>
         <v>27993.15923096902</v>
       </c>
-      <c r="L19" s="17">
-        <f>L13*$H$9</f>
+      <c r="L19" s="12">
+        <f>L14*$H$9</f>
         <v>22054.283059505222</v>
       </c>
-      <c r="M19" s="17">
-        <f>M13*$I$9</f>
+      <c r="M19" s="12">
+        <f>M14*$I$9</f>
         <v>19180.981613937325</v>
       </c>
-      <c r="N19" s="17">
+      <c r="N19" s="12">
         <f>N23-C20</f>
         <v>28148.829164055362</v>
       </c>
-      <c r="O19" s="17"/>
+      <c r="O19" s="12"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="17">
-        <f>K16*G9</f>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="12">
+        <f>K13*G9</f>
         <v>25431.55248336681</v>
       </c>
-      <c r="L20" s="17">
-        <f>L16*H9</f>
+      <c r="L20" s="12">
+        <f>L13*H9</f>
         <v>19875.470924748388</v>
       </c>
-      <c r="M20" s="17">
-        <f>M16*I9</f>
+      <c r="M20" s="12">
+        <f>M13*I9</f>
         <v>18236.374276418006</v>
       </c>
-      <c r="N20" s="17">
+      <c r="N20" s="12">
         <f>N24-C21</f>
         <v>27628.45544554455</v>
       </c>
-      <c r="O20" s="17"/>
+      <c r="O20" s="12"/>
     </row>
     <row r="21" spans="2:15" ht="16.2" x14ac:dyDescent="0.45">
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="22">
+      <c r="C21" s="17">
         <f>'[2]Balance Sheet'!$F$49</f>
         <v>2986</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="31" t="s">
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="L21" s="27"/>
-      <c r="M21" s="27"/>
-      <c r="N21" s="27"/>
-      <c r="O21" s="27"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
+      <c r="O21" s="22"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="23">
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="18">
         <f>K18-$C$21</f>
         <v>28446.446007031642</v>
       </c>
-      <c r="L22" s="23">
-        <f t="shared" ref="L22:M22" si="5">L18-$C$21</f>
+      <c r="L22" s="18">
+        <f t="shared" ref="L22:M22" si="1">L18-$C$21</f>
         <v>19051.30961923848</v>
       </c>
-      <c r="M22" s="23">
-        <f t="shared" si="5"/>
+      <c r="M22" s="18">
+        <f t="shared" si="1"/>
         <v>15307.4873110921</v>
       </c>
-      <c r="N22" s="23">
+      <c r="N22" s="18">
         <f>N26*$F$9</f>
         <v>27626.222693018626</v>
       </c>
-      <c r="O22" s="11"/>
+      <c r="O22" s="10"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="23">
-        <f t="shared" ref="K23:M23" si="6">K19-$C$21</f>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="18">
+        <f t="shared" ref="K23:M23" si="2">K19-$C$21</f>
         <v>25007.15923096902</v>
       </c>
-      <c r="L23" s="23">
-        <f t="shared" si="6"/>
+      <c r="L23" s="18">
+        <f t="shared" si="2"/>
         <v>19068.283059505222</v>
       </c>
-      <c r="M23" s="23">
-        <f t="shared" si="6"/>
+      <c r="M23" s="18">
+        <f t="shared" si="2"/>
         <v>16194.981613937325</v>
       </c>
-      <c r="N23" s="23">
+      <c r="N23" s="18">
         <f>N27*$F$9</f>
         <v>28148.829164055362</v>
       </c>
-      <c r="O23" s="11"/>
+      <c r="O23" s="10"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="23">
-        <f t="shared" ref="K24:M24" si="7">K20-$C$21</f>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="18">
+        <f t="shared" ref="K24:M24" si="3">K20-$C$21</f>
         <v>22445.55248336681</v>
       </c>
-      <c r="L24" s="23">
-        <f t="shared" si="7"/>
+      <c r="L24" s="18">
+        <f t="shared" si="3"/>
         <v>16889.470924748388</v>
       </c>
-      <c r="M24" s="23">
-        <f t="shared" si="7"/>
+      <c r="M24" s="18">
+        <f t="shared" si="3"/>
         <v>15250.374276418006</v>
       </c>
-      <c r="N24" s="23">
+      <c r="N24" s="18">
         <f>N28*$F$9</f>
         <v>30614.45544554455</v>
       </c>
-      <c r="O24" s="11"/>
+      <c r="O24" s="10"/>
     </row>
     <row r="25" spans="2:15" ht="16.2" x14ac:dyDescent="0.45">
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="L25" s="28"/>
-      <c r="M25" s="28"/>
-      <c r="N25" s="29"/>
-      <c r="O25" s="28"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="24"/>
+      <c r="O25" s="23"/>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="25">
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="20">
         <f>K22/$F$9*2</f>
         <v>64.946223760346214</v>
       </c>
-      <c r="L26" s="25">
+      <c r="L26" s="20">
         <f>L22/$F$9*2</f>
         <v>43.496140683192877</v>
       </c>
-      <c r="M26" s="25">
+      <c r="M26" s="20">
         <f>M22/$F$9*2</f>
         <v>34.948601166876941</v>
       </c>
-      <c r="N26" s="25">
+      <c r="N26" s="20">
         <f>N12*$O$9*2</f>
         <v>31.536783896139983</v>
       </c>
-      <c r="O26" s="24"/>
+      <c r="O26" s="19"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
-      <c r="K27" s="25">
-        <f t="shared" ref="K27:M28" si="8">K23/$F$9*2</f>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="20">
+        <f t="shared" ref="K27:M28" si="4">K23/$F$9*2</f>
         <v>57.093970846961234</v>
       </c>
-      <c r="L27" s="25">
-        <f t="shared" si="8"/>
+      <c r="L27" s="20">
+        <f t="shared" si="4"/>
         <v>43.534892829920601</v>
       </c>
-      <c r="M27" s="25">
-        <f t="shared" si="8"/>
+      <c r="M27" s="20">
+        <f t="shared" si="4"/>
         <v>36.974843867436817</v>
       </c>
-      <c r="N27" s="25">
-        <f t="shared" ref="N27:N28" si="9">N13*$O$9*2</f>
+      <c r="N27" s="20">
+        <f>N14*$O$9*2</f>
         <v>32.133366625633975</v>
       </c>
-      <c r="O27" s="24"/>
+      <c r="O27" s="19"/>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="K28" s="25">
-        <f t="shared" si="8"/>
+      <c r="K28" s="20">
+        <f t="shared" si="4"/>
         <v>51.245553614992716</v>
       </c>
-      <c r="L28" s="25">
-        <f t="shared" si="8"/>
+      <c r="L28" s="20">
+        <f t="shared" si="4"/>
         <v>38.560435901252028</v>
       </c>
-      <c r="M28" s="25">
-        <f t="shared" si="8"/>
+      <c r="M28" s="20">
+        <f t="shared" si="4"/>
         <v>34.818206110543393</v>
       </c>
-      <c r="N28" s="25">
-        <f t="shared" si="9"/>
+      <c r="N28" s="20">
+        <f>N15*$O$9*2</f>
         <v>34.948008499480082</v>
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="J29" s="33" t="s">
+      <c r="J29" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="K29" s="20">
+      <c r="K29" s="15">
         <f>AVERAGE(K26:K28)</f>
         <v>57.761916074100064</v>
       </c>
-      <c r="L29" s="20">
+      <c r="L29" s="15">
         <f>AVERAGE(L26:L28)</f>
         <v>41.86382313812183</v>
       </c>
-      <c r="M29" s="20">
-        <f t="shared" ref="L29:N29" si="10">AVERAGE(M26:M28)</f>
+      <c r="M29" s="15">
+        <f t="shared" ref="M29:N29" si="5">AVERAGE(M26:M28)</f>
         <v>35.580550381619048</v>
       </c>
-      <c r="N29" s="20">
-        <f t="shared" si="10"/>
+      <c r="N29" s="15">
+        <f t="shared" si="5"/>
         <v>32.872719673751348</v>
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="J30" s="33" t="s">
+      <c r="J30" s="28"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="J31" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="K30" s="34">
+      <c r="K31" s="29">
         <f>C9</f>
         <v>36.82</v>
       </c>
-      <c r="L30" s="34"/>
-      <c r="M30" s="34"/>
-      <c r="N30" s="34"/>
-      <c r="O30" s="35"/>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="J31" s="33" t="s">
+      <c r="L31" s="29"/>
+      <c r="M31" s="29"/>
+      <c r="N31" s="29"/>
+      <c r="O31" s="29"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="J32" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="K31" s="34">
-        <f>K29-$K$30</f>
+      <c r="K32" s="29">
+        <f>K29-$K$31</f>
         <v>20.941916074100064</v>
       </c>
-      <c r="L31" s="34">
-        <f t="shared" ref="L31:N31" si="11">L29-$K$30</f>
+      <c r="L32" s="29">
+        <f t="shared" ref="L32:N32" si="6">L29-$K$31</f>
         <v>5.0438231381218301</v>
       </c>
-      <c r="M31" s="34">
+      <c r="M32" s="29">
+        <f t="shared" si="6"/>
+        <v>-1.2394496183809522</v>
+      </c>
+      <c r="N32" s="29">
+        <f t="shared" si="6"/>
+        <v>-3.9472803262486522</v>
+      </c>
+      <c r="O32" s="29"/>
+    </row>
+    <row r="33" spans="10:15" x14ac:dyDescent="0.3">
+      <c r="J33" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="K33" s="30">
+        <f>K32/$K$31</f>
+        <v>0.56876469511407013</v>
+      </c>
+      <c r="L33" s="30">
+        <f t="shared" ref="L33:N33" si="7">L32/$K$31</f>
+        <v>0.13698596246935987</v>
+      </c>
+      <c r="M33" s="31">
+        <f t="shared" si="7"/>
+        <v>-3.3662401368303972E-2</v>
+      </c>
+      <c r="N33" s="31">
+        <f t="shared" si="7"/>
+        <v>-0.1072047888715006</v>
+      </c>
+      <c r="O33" s="29"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F0123B3-D1D9-4C5A-957B-0A66B96211D1}">
+  <dimension ref="B2:M32"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:13" ht="16.2" x14ac:dyDescent="0.45">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+    </row>
+    <row r="3" spans="2:13" ht="16.2" x14ac:dyDescent="0.45">
+      <c r="B3" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="7">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B4" s="32">
+        <v>43586</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4">
+        <v>6700</v>
+      </c>
+      <c r="E4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="39">
+        <f>D4/1500</f>
+        <v>4.4666666666666668</v>
+      </c>
+      <c r="G4" s="39">
+        <f>D4/441</f>
+        <v>15.192743764172336</v>
+      </c>
+      <c r="H4" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="7">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B5" s="32">
+        <v>42795</v>
+      </c>
+      <c r="C5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5">
+        <v>2740</v>
+      </c>
+      <c r="E5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="39">
+        <f>D5/(850*K3)</f>
+        <v>2.7789046653144021</v>
+      </c>
+      <c r="G5" s="39">
+        <f>D5/(210*K3)</f>
+        <v>11.247947454844008</v>
+      </c>
+      <c r="H5" s="39" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B6" s="32">
+        <v>43770</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6">
+        <v>5400</v>
+      </c>
+      <c r="E6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="39">
+        <f>D6/920.9</f>
+        <v>5.8638288630687372</v>
+      </c>
+      <c r="G6" s="39">
+        <f>D6/160</f>
+        <v>33.75</v>
+      </c>
+      <c r="H6" s="39">
+        <f>D6/11.6</f>
+        <v>465.51724137931035</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B7" s="32">
+        <v>44440</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7">
+        <v>12400</v>
+      </c>
+      <c r="E7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="39">
+        <v>4.3</v>
+      </c>
+      <c r="G7" s="39">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="H7" s="39">
+        <f>D7/400.2</f>
+        <v>30.984507746126937</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B8" s="32">
+        <v>45323</v>
+      </c>
+      <c r="C8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8">
+        <v>1500</v>
+      </c>
+      <c r="E8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="39">
+        <v>3.97</v>
+      </c>
+      <c r="G8" s="39">
+        <v>15.7</v>
+      </c>
+      <c r="H8" s="39">
+        <f>D8/69</f>
+        <v>21.739130434782609</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B9" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="40">
+        <f>AVERAGE(F4:F8)</f>
+        <v>4.2758800390099605</v>
+      </c>
+      <c r="G9" s="40">
+        <f>AVERAGE(G4:G8)</f>
+        <v>19.09813824380327</v>
+      </c>
+      <c r="H9" s="40">
+        <f>AVERAGE(H4:H5,H7:H8)</f>
+        <v>26.361819090454773</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B10" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="40">
+        <f>HARMEAN(F4:F8)</f>
+        <v>4.0364280952852667</v>
+      </c>
+      <c r="G10" s="40">
+        <f>HARMEAN(G4:G8)</f>
+        <v>16.718476650677161</v>
+      </c>
+      <c r="H10" s="40">
+        <f>HARMEAN(H4:H5,H7:H8)</f>
+        <v>25.551205439934058</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B11" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="40">
+        <f>MEDIAN(F4:F8)</f>
+        <v>4.3</v>
+      </c>
+      <c r="G11" s="40">
+        <f>MEDIAN(G4:G8)</f>
+        <v>15.7</v>
+      </c>
+      <c r="H11" s="40">
+        <f>MEDIAN(H4:H5,H7:H8)</f>
+        <v>26.361819090454773</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" ht="16.2" x14ac:dyDescent="0.45">
+      <c r="B13" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+    </row>
+    <row r="14" spans="2:13" ht="16.2" x14ac:dyDescent="0.45">
+      <c r="B14" s="41"/>
+      <c r="C14" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="41" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="14">
+        <f>[1]DCF!$I$9</f>
+        <v>36.82</v>
+      </c>
+      <c r="D15" s="13">
+        <f>'[2]Income Statement'!$F$25</f>
+        <v>876</v>
+      </c>
+      <c r="E15" s="13">
+        <f>'[2]Balance Sheet'!$F$49</f>
+        <v>2986</v>
+      </c>
+      <c r="F15" s="13">
+        <f>'[2]Income Statement'!$F$2</f>
+        <v>5810</v>
+      </c>
+      <c r="G15" s="13">
+        <f>'[2]Income Statement'!$F$40</f>
+        <v>1335</v>
+      </c>
+      <c r="H15" s="13">
+        <f>'[2]Income Statement'!$F$8</f>
+        <v>886</v>
+      </c>
+      <c r="I15" s="13"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="35"/>
+    </row>
+    <row r="16" spans="2:13" ht="16.2" x14ac:dyDescent="0.45">
+      <c r="F16" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="42">
+        <f>F$15*F9</f>
+        <v>24842.863026647872</v>
+      </c>
+      <c r="G17" s="42">
+        <f t="shared" ref="G17:H17" si="0">G$15*G9</f>
+        <v>25496.014555477366</v>
+      </c>
+      <c r="H17" s="42">
+        <f t="shared" si="0"/>
+        <v>23356.57171414293</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="42">
+        <f t="shared" ref="F18:H18" si="1">F$15*F10</f>
+        <v>23451.6472336074</v>
+      </c>
+      <c r="G18" s="42">
+        <f t="shared" si="1"/>
+        <v>22319.16632865401</v>
+      </c>
+      <c r="H18" s="42">
+        <f t="shared" si="1"/>
+        <v>22638.368019781577</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="42">
+        <f t="shared" ref="F19:H19" si="2">F$15*F11</f>
+        <v>24983</v>
+      </c>
+      <c r="G19" s="42">
+        <f t="shared" si="2"/>
+        <v>20959.5</v>
+      </c>
+      <c r="H19" s="42">
+        <f t="shared" si="2"/>
+        <v>23356.57171414293</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="16.2" x14ac:dyDescent="0.45">
+      <c r="F20" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="42">
+        <f>F17-$E$15</f>
+        <v>21856.863026647872</v>
+      </c>
+      <c r="G21" s="42">
+        <f t="shared" ref="G21:H21" si="3">G17-$E$15</f>
+        <v>22510.014555477366</v>
+      </c>
+      <c r="H21" s="42">
+        <f t="shared" si="3"/>
+        <v>20370.57171414293</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" s="42">
+        <f t="shared" ref="F22:H22" si="4">F18-$E$15</f>
+        <v>20465.6472336074</v>
+      </c>
+      <c r="G22" s="42">
+        <f t="shared" si="4"/>
+        <v>19333.16632865401</v>
+      </c>
+      <c r="H22" s="42">
+        <f t="shared" si="4"/>
+        <v>19652.368019781577</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="42">
+        <f t="shared" ref="F23:H23" si="5">F19-$E$15</f>
+        <v>21997</v>
+      </c>
+      <c r="G23" s="42">
+        <f t="shared" si="5"/>
+        <v>17973.5</v>
+      </c>
+      <c r="H23" s="42">
+        <f t="shared" si="5"/>
+        <v>20370.57171414293</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="16.2" x14ac:dyDescent="0.45">
+      <c r="F24" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="15">
+        <f>F21/$D$15</f>
+        <v>24.950756879735014</v>
+      </c>
+      <c r="G25" s="15">
+        <f t="shared" ref="G25:H25" si="6">G21/$D$15</f>
+        <v>25.696363647805214</v>
+      </c>
+      <c r="H25" s="15">
+        <f t="shared" si="6"/>
+        <v>23.254077299249921</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26" s="15">
+        <f t="shared" ref="F26:H26" si="7">F22/$D$15</f>
+        <v>23.362610997268721</v>
+      </c>
+      <c r="G26" s="15">
+        <f t="shared" si="7"/>
+        <v>22.069824576089051</v>
+      </c>
+      <c r="H26" s="15">
+        <f t="shared" si="7"/>
+        <v>22.434210068243811</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" s="15">
+        <f t="shared" ref="F27:H27" si="8">F23/$D$15</f>
+        <v>25.110730593607308</v>
+      </c>
+      <c r="G27" s="15">
+        <f t="shared" si="8"/>
+        <v>20.517694063926939</v>
+      </c>
+      <c r="H27" s="15">
+        <f t="shared" si="8"/>
+        <v>23.254077299249921</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E28" t="s">
+        <v>64</v>
+      </c>
+      <c r="F28" s="15">
+        <f>AVERAGE(F25:F27)</f>
+        <v>24.47469949020368</v>
+      </c>
+      <c r="G28" s="15">
+        <f>AVERAGE(G25:G27)</f>
+        <v>22.7612940959404</v>
+      </c>
+      <c r="H28" s="15">
+        <f>AVERAGE(H25:H27)</f>
+        <v>22.980788222247885</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E30" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="F30" s="29">
+        <f>C15</f>
+        <v>36.82</v>
+      </c>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E31" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="F31" s="29">
+        <f>F28-$F$30</f>
+        <v>-12.345300509796321</v>
+      </c>
+      <c r="G31" s="29">
+        <f t="shared" ref="G31:H31" si="9">G28-$F$30</f>
+        <v>-14.0587059040596</v>
+      </c>
+      <c r="H31" s="29">
+        <f t="shared" si="9"/>
+        <v>-13.839211777752116</v>
+      </c>
+      <c r="I31" s="29">
+        <f t="shared" ref="G31:I31" si="10">I28-$K$30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E32" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="F32" s="31">
+        <f>F31/F28</f>
+        <v>-0.50441070848439584</v>
+      </c>
+      <c r="G32" s="31">
+        <f t="shared" ref="G32:H32" si="11">G31/G28</f>
+        <v>-0.61765846198380459</v>
+      </c>
+      <c r="H32" s="31">
         <f t="shared" si="11"/>
-        <v>-1.2394496183809522</v>
-      </c>
-      <c r="N31" s="34">
-        <f t="shared" si="11"/>
-        <v>-3.9472803262486522</v>
-      </c>
-      <c r="O31" s="35"/>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="J32" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="K32" s="36">
-        <f>K31/$K$30</f>
-        <v>0.56876469511407013</v>
-      </c>
-      <c r="L32" s="36">
-        <f t="shared" ref="L32:N32" si="12">L31/$K$30</f>
-        <v>0.13698596246935987</v>
-      </c>
-      <c r="M32" s="36">
-        <f t="shared" si="12"/>
-        <v>-3.3662401368303972E-2</v>
-      </c>
-      <c r="N32" s="36">
-        <f t="shared" si="12"/>
-        <v>-0.1072047888715006</v>
-      </c>
-      <c r="O32" s="35"/>
+        <v>-0.60220788094440836</v>
+      </c>
+      <c r="I32" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>